<commit_message>
buggy table is added, error in mitarbeiterKosten.tex
</commit_message>
<xml_diff>
--- a/excelData.xlsx
+++ b/excelData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucliss/Documents/repos/rechnungSkript/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucliss/Documents/repos/rechnungMARSters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A296E8F-B80E-5949-B2D0-A80548100AFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25DECCA9-30DB-114E-9CAF-9F7FD5355751}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6780" yWindow="7720" windowWidth="27640" windowHeight="16860" xr2:uid="{D3EC4FF9-2BB6-2944-B9C2-FA9566BC8D6A}"/>
+    <workbookView xWindow="1760" yWindow="2260" windowWidth="27640" windowHeight="16860" xr2:uid="{D3EC4FF9-2BB6-2944-B9C2-FA9566BC8D6A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -251,9 +251,6 @@
     <t>Netzwerktechnik-Spezialist</t>
   </si>
   <si>
-    <t>Projektleitung &amp; Planung</t>
-  </si>
-  <si>
     <t>Hardwareinstallation (Roboterteam)</t>
   </si>
   <si>
@@ -261,6 +258,9 @@
   </si>
   <si>
     <t>Summe netto</t>
+  </si>
+  <si>
+    <t>Projektleitung und Planung</t>
   </si>
 </sst>
 </file>
@@ -671,12 +671,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -689,6 +683,12 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="6" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1032,8 +1032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4358DD47-7E6D-DD40-92A6-39C8C7C2E111}">
   <dimension ref="A4:I79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="143" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="143" workbookViewId="0">
+      <selection activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1061,18 +1061,18 @@
       <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="42" t="s">
+      <c r="C6" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="42"/>
-      <c r="E6" s="43" t="s">
+      <c r="D6" s="48"/>
+      <c r="E6" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="43"/>
-      <c r="H6" s="44" t="s">
+      <c r="F6" s="49"/>
+      <c r="H6" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="I6" s="44" t="s">
+      <c r="I6" s="42" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1089,10 +1089,10 @@
       <c r="F7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H7" s="44" t="s">
+      <c r="H7" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="I7" s="44" t="s">
+      <c r="I7" s="42" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1110,10 +1110,10 @@
         <f>H72 *1.2</f>
         <v>10080</v>
       </c>
-      <c r="H8" s="44" t="s">
+      <c r="H8" s="42" t="s">
         <v>63</v>
       </c>
-      <c r="I8" s="44" t="s">
+      <c r="I8" s="42" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1221,14 +1221,14 @@
       <c r="A21" t="s">
         <v>1</v>
       </c>
-      <c r="C21" s="42" t="s">
+      <c r="C21" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="D21" s="42"/>
-      <c r="E21" s="43" t="s">
+      <c r="D21" s="48"/>
+      <c r="E21" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="F21" s="43"/>
+      <c r="F21" s="49"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
@@ -1812,16 +1812,16 @@
       <c r="H73" s="41"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A74" s="45" t="s">
+      <c r="A74" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="B74" s="45" t="s">
+      <c r="B74" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="C74" s="45" t="s">
+      <c r="C74" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="D74" s="45" t="s">
+      <c r="D74" s="43" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1829,71 +1829,71 @@
       <c r="A75" t="s">
         <v>70</v>
       </c>
-      <c r="B75" s="46">
+      <c r="B75" s="44">
         <v>150</v>
       </c>
-      <c r="C75" s="47">
+      <c r="C75" s="45">
         <v>1200</v>
       </c>
-      <c r="D75" s="47">
+      <c r="D75" s="45">
         <f>B75*C75</f>
         <v>180000</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>71</v>
-      </c>
-      <c r="B76" s="46">
-        <v>80</v>
-      </c>
-      <c r="C76" s="46">
+        <v>74</v>
+      </c>
+      <c r="B76" s="44">
+        <v>85</v>
+      </c>
+      <c r="C76" s="44">
         <v>900</v>
       </c>
-      <c r="D76" s="47">
+      <c r="D76" s="45">
         <f>B76*C76</f>
-        <v>72000</v>
+        <v>76500</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>72</v>
-      </c>
-      <c r="B77" s="46">
+        <v>71</v>
+      </c>
+      <c r="B77" s="44">
         <v>300</v>
       </c>
-      <c r="C77" s="46">
+      <c r="C77" s="44">
         <v>600</v>
       </c>
-      <c r="D77" s="47">
+      <c r="D77" s="45">
         <f>B77*C77</f>
         <v>180000</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>73</v>
-      </c>
-      <c r="B78" s="46">
+        <v>72</v>
+      </c>
+      <c r="B78" s="44">
         <v>200</v>
       </c>
-      <c r="C78" s="47">
+      <c r="C78" s="45">
         <v>1000</v>
       </c>
-      <c r="D78" s="47">
+      <c r="D78" s="45">
         <f>B78*C78</f>
         <v>200000</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A79" s="48" t="s">
-        <v>74</v>
-      </c>
-      <c r="B79" s="46"/>
-      <c r="C79" s="46"/>
-      <c r="D79" s="49">
+      <c r="A79" s="46" t="s">
+        <v>73</v>
+      </c>
+      <c r="B79" s="44"/>
+      <c r="C79" s="44"/>
+      <c r="D79" s="47">
         <f>D75+D76+D77+D78</f>
-        <v>632000</v>
+        <v>636500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
defined output folder and implemented os command execution
</commit_message>
<xml_diff>
--- a/excelData.xlsx
+++ b/excelData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucliss/Documents/repos/rechnungMARSters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50BCA362-E018-E14E-A2F4-AD43AF66B018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1F6E6A3-0468-B34D-8E48-E51C4397F5F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4920" yWindow="2860" windowWidth="27640" windowHeight="16860" xr2:uid="{D3EC4FF9-2BB6-2944-B9C2-FA9566BC8D6A}"/>
   </bookViews>
@@ -1035,8 +1035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4358DD47-7E6D-DD40-92A6-39C8C7C2E111}">
   <dimension ref="A4:I79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="143" workbookViewId="0">
-      <selection activeCell="F76" sqref="F76"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="143" workbookViewId="0">
+      <selection activeCell="F79" sqref="F79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>